<commit_message>
Ya'll wanted some updates?
</commit_message>
<xml_diff>
--- a/unlocks.xlsx
+++ b/unlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Stuff\Games\Games\The Binding of Isaac Rebirth Repentance\mods\Dies Irae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AA1517-58C2-4925-BACD-A6863594557D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B162EBD3-B978-45DE-AB2E-23FACE769DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{749A19A5-9F47-4779-B35D-46566BE7EDBF}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{749A19A5-9F47-4779-B35D-46566BE7EDBF}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="125">
   <si>
     <t>Unlock</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Ultra secret map</t>
   </si>
   <si>
-    <t>Visit to different ultra secret rooms in a single run</t>
-  </si>
-  <si>
     <t>Traveler logbook</t>
   </si>
   <si>
@@ -403,6 +400,15 @@
   </si>
   <si>
     <t>Lose all heart containers with Maggie</t>
+  </si>
+  <si>
+    <t>Visit two different ultra secret rooms in a single run</t>
+  </si>
+  <si>
+    <t>Dad's empty wallet</t>
+  </si>
+  <si>
+    <t>Defeat a random modded enemy with Keeper</t>
   </si>
 </sst>
 </file>
@@ -797,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8416C38A-7BDB-431A-9A43-48F1122F9F29}">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -906,14 +912,14 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>92</v>
+      <c r="C10" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
@@ -939,14 +945,14 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>92</v>
+      <c r="C13" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -968,7 +974,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
@@ -1012,7 +1018,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
@@ -1023,7 +1029,7 @@
         <v>38</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
@@ -1034,7 +1040,7 @@
         <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
@@ -1067,419 +1073,419 @@
         <v>38</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>30</v>
@@ -1488,30 +1494,36 @@
     </row>
     <row r="63" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+    </row>
+    <row r="65" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>

</xml_diff>

<commit_message>
Some items works, some needs works
</commit_message>
<xml_diff>
--- a/unlocks.xlsx
+++ b/unlocks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Stuff\Games\Games\The Binding of Isaac Rebirth Repentance\mods\Dies Irae\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Stuff\Apps\Steam\steamapps\common\The Binding of Isaac Rebirth\mods\Dies Irae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B162EBD3-B978-45DE-AB2E-23FACE769DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2E00DB-F056-486B-B0E3-71DD98F7703F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{749A19A5-9F47-4779-B35D-46566BE7EDBF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{749A19A5-9F47-4779-B35D-46566BE7EDBF}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8416C38A-7BDB-431A-9A43-48F1122F9F29}">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>